<commit_message>
state specific fix (#46)
</commit_message>
<xml_diff>
--- a/requirement/src/main/resources/templates/BizFinReview.xlsx
+++ b/requirement/src/main/resources/templates/BizFinReview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>IPC Proposed Quantity</t>
   </si>
   <si>
-    <t>CDO Override reason</t>
-  </si>
-  <si>
     <t>BizFin Quantity Recommendation</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Procurement Type</t>
+  </si>
+  <si>
+    <t>CDO Override Reason</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,7 @@
   <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+      <selection activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -541,28 +541,28 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>10</v>
@@ -574,10 +574,10 @@
         <v>12</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>13</v>
@@ -604,13 +604,13 @@
         <v>20</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data validation in templates
</commit_message>
<xml_diff>
--- a/requirement/src/main/resources/templates/BizFinReview.xlsx
+++ b/requirement/src/main/resources/templates/BizFinReview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,8 @@
   <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="3" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -640,8 +641,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="Bizfin Quantity Recommendation should be number" sqref="AH1:AH1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
data validation in templates (#95)
</commit_message>
<xml_diff>
--- a/requirement/src/main/resources/templates/BizFinReview.xlsx
+++ b/requirement/src/main/resources/templates/BizFinReview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -527,7 +527,8 @@
   <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane xSplit="3" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -640,8 +641,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Data" error="Bizfin Quantity Recommendation should be number" sqref="AH1:AH1048576">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>